<commit_message>
Added Eluta and workopolis support
</commit_message>
<xml_diff>
--- a/Applications.xlsx
+++ b/Applications.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
-  <si>
-    <t>2020-05-19</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="27">
+  <si>
+    <t>2020-05-20</t>
   </si>
   <si>
     <t>Web Developer Intern</t>
@@ -31,6 +31,17 @@
     <t>Full Time Grocery Clerk</t>
   </si>
   <si>
+    <t>Immigration Consultant</t>
+  </si>
+  <si>
+    <t>Architectural Technologist/Intern Architect (Junior &amp; Intermediate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Registered Massage Therapist (RMT)
+</t>
+  </si>
+  <si>
     <t>Pathcore</t>
   </si>
   <si>
@@ -43,6 +54,17 @@
     <t>Metro Inc.</t>
   </si>
   <si>
+    <t>Green Light Canada Global Mobility Solutions</t>
+  </si>
+  <si>
+    <t>CORE ARCHITECTS INC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Hammam Spa Inc.
+</t>
+  </si>
+  <si>
     <t>https://ca.indeed.com/viewjob?jk=45e7adfb4d34664e&amp;tk=1e8k9749r0gc1000&amp;from=serp&amp;vjs=3</t>
   </si>
   <si>
@@ -53,6 +75,18 @@
   </si>
   <si>
     <t>https://ca.linkedin.com/jobs/view/full-time-grocery-clerk-at-metro-inc-1745872580?refId=36c2798d-7978-49ff-b53b-8350dd36c1cb&amp;position=2&amp;pageNum=0&amp;trk=public_jobs_job-result-card_result-card_full-click</t>
+  </si>
+  <si>
+    <t>https://www.workopolis.com/jobsearch/viewjob/t6EaVFpXCXm9ef_kIrlCueqgBpIKnq-WGzdfh4IIQvj67EENxQIuTw?ak=intern&amp;l=Toronto%2C+ON&amp;isp=1</t>
+  </si>
+  <si>
+    <t>https://www.workopolis.com/jobsearch/viewjob/tdsUdvHgShbWaCWvIxgz1CpR8ywq-eUELT05jixFzeP9wzsQNYParw?ak=intern&amp;l=Toronto%2C+ON&amp;isp=1</t>
+  </si>
+  <si>
+    <t>https://job-openings.monster.ca/public-relations-internship-kirkland-lake-on-ca-englehart-district-hospital/217713535</t>
+  </si>
+  <si>
+    <t>https://www.eluta.ca/spl/registered-massage-therapist-rmt-21a55bb92ef26470a6dd211bd9828797?imo=11</t>
   </si>
   <si>
     <t>Date</t>
@@ -436,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,16 +484,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -473,10 +507,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -490,10 +524,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -507,10 +541,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -524,10 +558,400 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2">
         <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -536,6 +960,30 @@
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
     <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
+    <hyperlink ref="E12" r:id="rId11"/>
+    <hyperlink ref="E13" r:id="rId12"/>
+    <hyperlink ref="E14" r:id="rId13"/>
+    <hyperlink ref="E15" r:id="rId14"/>
+    <hyperlink ref="E16" r:id="rId15"/>
+    <hyperlink ref="E17" r:id="rId16"/>
+    <hyperlink ref="E18" r:id="rId17"/>
+    <hyperlink ref="E19" r:id="rId18"/>
+    <hyperlink ref="E20" r:id="rId19"/>
+    <hyperlink ref="E21" r:id="rId20"/>
+    <hyperlink ref="E22" r:id="rId21"/>
+    <hyperlink ref="E23" r:id="rId22"/>
+    <hyperlink ref="E24" r:id="rId23"/>
+    <hyperlink ref="E25" r:id="rId24"/>
+    <hyperlink ref="E26" r:id="rId25"/>
+    <hyperlink ref="E27" r:id="rId26"/>
+    <hyperlink ref="E28" r:id="rId27"/>
+    <hyperlink ref="E29" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added more information to timeline
</commit_message>
<xml_diff>
--- a/Applications.xlsx
+++ b/Applications.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="17">
   <si>
     <t>2020-05-21</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">Python HTML CSS Javascript Java C++ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTML CSS Javascript Java C++ Objective c GIT Swift </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python HTML CSS Javascript Java GIT </t>
   </si>
   <si>
     <t>https://www.linkedin.com/jobs/view/1865907079/?eBP=JYMBII_JOBS_HOME_ORGANIC&amp;recommendedFlavor=SCHOOL_RECRUIT&amp;refId=f6e15b88-0061-4368-b3ce-fe439cee172c&amp;trk=d_flagship3_jobs_discovery_jymbii</t>
@@ -430,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,19 +450,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -476,7 +482,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -496,7 +502,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -516,7 +522,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -536,7 +542,207 @@
         <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
         <v>9</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -545,6 +751,16 @@
     <hyperlink ref="F3" r:id="rId2"/>
     <hyperlink ref="F4" r:id="rId3"/>
     <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F11" r:id="rId10"/>
+    <hyperlink ref="F12" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId12"/>
+    <hyperlink ref="F14" r:id="rId13"/>
+    <hyperlink ref="F15" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improved memory effeciency of excel class
</commit_message>
<xml_diff>
--- a/Applications.xlsx
+++ b/Applications.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>2020-06-04</t>
   </si>
@@ -64,13 +64,13 @@
     <t>Toronto, Ontario, Canada</t>
   </si>
   <si>
-    <t xml:space="preserve">Python HTML CSS Javascript Java GIT REST </t>
+    <t xml:space="preserve">Python HTML CSS Javascript Java C++ GIT REST </t>
   </si>
   <si>
     <t xml:space="preserve">Python HTML CSS Javascript Java PHP MySQL Scala JQuery Ajax AWS REST </t>
   </si>
   <si>
-    <t xml:space="preserve">Python HTML CSS Javascript Java C++ GIT Bootstrap ReactJS AWS Azure Kubernetes REST </t>
+    <t xml:space="preserve">Python HTML CSS Javascript Java GIT Bootstrap ReactJS AWS Azure Kubernetes REST </t>
   </si>
   <si>
     <t xml:space="preserve">Python Javascript Java GIT Kotlin Azure REST </t>
@@ -80,15 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">HTML CSS Javascript Java GIT PHP MySQL Scala JQuery MVC MVP MVVM REST JAX-RS XML-RPC JSON-RPC SOAP JDBC MKS FuelCMS CodeIgniter </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python HTML CSS Javascript Java C++ GIT REST </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python HTML CSS Javascript Java GIT Bootstrap ReactJS AWS Azure Kubernetes REST </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python HTML CSS Javascript Java C++ GIT PHP MySQL Scala JQuery Ajax AWS REST </t>
   </si>
   <si>
     <t>https://www.linkedin.com/jobs/view/1865907079/?eBP=JYMBII_JOBS_HOME_ORGANIC&amp;recommendedFlavor=SCHOOL_RECRUIT&amp;refId=f6e15b88-0061-4368-b3ce-fe439cee172c&amp;trk=d_flagship3_jobs_discovery_jymbii</t>
@@ -507,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -522,22 +513,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -556,8 +547,11 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -580,7 +574,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -603,7 +597,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -620,13 +614,13 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -649,7 +643,7 @@
         <v>19</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -672,7 +666,7 @@
         <v>20</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -695,327 +689,11 @@
         <v>21</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="3" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:F22">
+  <conditionalFormatting sqref="C1:F8">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Not found">
       <formula>NOT(ISERROR(SEARCH("Not found",C1)))</formula>
     </cfRule>
@@ -1028,20 +706,6 @@
     <hyperlink ref="G6" r:id="rId5"/>
     <hyperlink ref="G7" r:id="rId6"/>
     <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G9" r:id="rId8"/>
-    <hyperlink ref="G10" r:id="rId9"/>
-    <hyperlink ref="G11" r:id="rId10"/>
-    <hyperlink ref="G12" r:id="rId11"/>
-    <hyperlink ref="G13" r:id="rId12"/>
-    <hyperlink ref="G14" r:id="rId13"/>
-    <hyperlink ref="G15" r:id="rId14"/>
-    <hyperlink ref="G16" r:id="rId15"/>
-    <hyperlink ref="G17" r:id="rId16"/>
-    <hyperlink ref="G18" r:id="rId17"/>
-    <hyperlink ref="G19" r:id="rId18"/>
-    <hyperlink ref="G20" r:id="rId19"/>
-    <hyperlink ref="G21" r:id="rId20"/>
-    <hyperlink ref="G22" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added functions to handle invalid urls
</commit_message>
<xml_diff>
--- a/Applications.xlsx
+++ b/Applications.xlsx
@@ -14,50 +14,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
-  <si>
-    <t>2020-06-04</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+  <si>
+    <t>2020-06-05</t>
+  </si>
+  <si>
+    <t>Web Developer Intern</t>
+  </si>
+  <si>
+    <t>Web Application Developer with Great Company</t>
+  </si>
+  <si>
+    <t>Front End Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android Engineer </t>
+  </si>
+  <si>
+    <t>Software Developer Intern</t>
+  </si>
+  <si>
+    <t>Full Stack PHP Developer 5+ years Experience Required</t>
+  </si>
+  <si>
+    <t>Pathcore</t>
+  </si>
+  <si>
+    <t>Vocalmeet</t>
+  </si>
+  <si>
+    <t>Lyncwork</t>
+  </si>
+  <si>
+    <t>Flipp</t>
+  </si>
+  <si>
+    <t>Konrad Group</t>
+  </si>
+  <si>
+    <t>Mainstream Media Unplugged Ltd.</t>
   </si>
   <si>
     <t>Not found</t>
   </si>
   <si>
-    <t>Web Developer Intern</t>
-  </si>
-  <si>
-    <t>Web Application Developer with Great Company</t>
-  </si>
-  <si>
-    <t>Front End Developer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android Engineer </t>
-  </si>
-  <si>
-    <t>Software Developer Intern</t>
-  </si>
-  <si>
-    <t>Full Stack PHP Developer 5+ years Experience Required</t>
-  </si>
-  <si>
-    <t>Pathcore</t>
-  </si>
-  <si>
-    <t>Vocalmeet</t>
-  </si>
-  <si>
-    <t>Lyncwork</t>
-  </si>
-  <si>
-    <t>Flipp</t>
-  </si>
-  <si>
-    <t>Konrad Group</t>
-  </si>
-  <si>
-    <t>Mainstream Media Unplugged Ltd.</t>
-  </si>
-  <si>
     <t>Toronto, ON</t>
   </si>
   <si>
@@ -70,19 +70,16 @@
     <t xml:space="preserve">Python HTML CSS Javascript Java PHP MySQL Scala JQuery Ajax AWS REST </t>
   </si>
   <si>
-    <t xml:space="preserve">Python HTML CSS Javascript Java GIT Bootstrap ReactJS AWS Azure Kubernetes REST </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python Javascript Java GIT Kotlin Azure REST </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTML CSS Javascript Java GIT </t>
+    <t xml:space="preserve">Python HTML CSS Javascript Java C++ GIT Bootstrap ReactJS AWS Azure Kubernetes REST </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python Javascript Java GIT PHP Kotlin Azure REST </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTML CSS Javascript Java GIT REST </t>
   </si>
   <si>
     <t xml:space="preserve">HTML CSS Javascript Java GIT PHP MySQL Scala JQuery MVC MVP MVVM REST JAX-RS XML-RPC JSON-RPC SOAP JDBC MKS FuelCMS CodeIgniter </t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/jobs/view/1865907079/?eBP=JYMBII_JOBS_HOME_ORGANIC&amp;recommendedFlavor=SCHOOL_RECRUIT&amp;refId=f6e15b88-0061-4368-b3ce-fe439cee172c&amp;trk=d_flagship3_jobs_discovery_jymbii</t>
   </si>
   <si>
     <t>https://ca.indeed.com/viewjob?jk=45e7adfb4d34664e&amp;tk=1e8k9749r0gc1000&amp;from=serp&amp;vjs=3</t>
@@ -149,12 +146,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF919190"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -190,7 +193,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -204,7 +207,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFE84A3F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -498,37 +501,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="7" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -542,13 +543,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>22</v>
@@ -568,10 +569,10 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>23</v>
@@ -594,7 +595,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>24</v>
@@ -614,10 +615,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>25</v>
@@ -640,7 +641,7 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>26</v>
@@ -660,40 +661,17 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:F8">
+  <conditionalFormatting sqref="C1:F7">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Not found">
       <formula>NOT(ISERROR(SEARCH("Not found",C1)))</formula>
     </cfRule>
@@ -705,7 +683,6 @@
     <hyperlink ref="G5" r:id="rId4"/>
     <hyperlink ref="G6" r:id="rId5"/>
     <hyperlink ref="G7" r:id="rId6"/>
-    <hyperlink ref="G8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added graphing for activity and application distribution by company
</commit_message>
<xml_diff>
--- a/Applications.xlsx
+++ b/Applications.xlsx
@@ -14,90 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
-  <si>
-    <t>2020-06-05</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="15">
   <si>
     <t>Web Developer Intern</t>
   </si>
   <si>
-    <t>Web Application Developer with Great Company</t>
-  </si>
-  <si>
-    <t>Front End Developer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android Engineer </t>
-  </si>
-  <si>
-    <t>Software Developer Intern</t>
-  </si>
-  <si>
-    <t>Full Stack PHP Developer 5+ years Experience Required</t>
+    <t>Microsoft</t>
   </si>
   <si>
     <t>Pathcore</t>
   </si>
   <si>
-    <t>Vocalmeet</t>
+    <t>Google</t>
   </si>
   <si>
-    <t>Lyncwork</t>
-  </si>
-  <si>
-    <t>Flipp</t>
-  </si>
-  <si>
-    <t>Konrad Group</t>
-  </si>
-  <si>
-    <t>Mainstream Media Unplugged Ltd.</t>
+    <t>Toronto, ON</t>
   </si>
   <si>
     <t>Not found</t>
   </si>
   <si>
-    <t>Toronto, ON</t>
-  </si>
-  <si>
-    <t>Toronto, Ontario, Canada</t>
-  </si>
-  <si>
     <t xml:space="preserve">Python HTML CSS Javascript Java C++ GIT REST </t>
   </si>
   <si>
-    <t xml:space="preserve">Python HTML CSS Javascript Java PHP MySQL Scala JQuery Ajax AWS REST </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python HTML CSS Javascript Java C++ GIT Bootstrap ReactJS AWS Azure Kubernetes REST </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python Javascript Java GIT PHP Kotlin Azure REST </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTML CSS Javascript Java GIT REST </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTML CSS Javascript Java GIT PHP MySQL Scala JQuery MVC MVP MVVM REST JAX-RS XML-RPC JSON-RPC SOAP JDBC MKS FuelCMS CodeIgniter </t>
+    <t xml:space="preserve">Python HTML CSS Javascript Java GIT REST </t>
   </si>
   <si>
     <t>https://ca.indeed.com/viewjob?jk=45e7adfb4d34664e&amp;tk=1e8k9749r0gc1000&amp;from=serp&amp;vjs=3</t>
-  </si>
-  <si>
-    <t>https://ca.indeed.com/viewjob?cmp=Vocalmeet&amp;t=Web+Application+Developer+Great+Company&amp;jk=7b1ac7e5eec244ee&amp;sjdu=Kn_ZDJQRugQBtOoubfH7EF7nFJ6ehZcQtAxR8RFw7KQxyvngv5OIFpVtbgsjGQDS&amp;tk=1e9kdeec54f0k800&amp;adid=346533071&amp;pub=4a1b367933fd867b19b072952f68dceb&amp;vjs=3</t>
-  </si>
-  <si>
-    <t>https://ca.indeed.com/viewjob?cmp=Lyncwork&amp;t=Front+End+Developer&amp;jk=d503ac852a8e0a8b&amp;q=software&amp;vjs=3</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/jobs/view/1858231312/?eBP=CwEAAAFyaNupTyRdYL6rkkNQhf096BxM_KPMc4wXwu0hn7obFj7pi1vbtrTXy4RSj17cqBS8V1IxZcuV67Nr1PppW7l9e3ydgivujI1Lcrx-yfYJ0G0nSr69cEezdYWFu6HirCq8EvVf2f-oF3iZNCr_qgK2ZCKILMJ9DE7bljEJd5zvWK9v7oVyTywPMYzg4URoY8KxVGrDUjmHwIpid3rSLjqMxznyWdIKZLWQR5czUGmaSCLeOSNOXMqSCcOXU9ZzCFKiRxJ7g7lGMWOo-bnadgfQTxu4sHcIdtzci378VAjJMjnLStiUkh8pq8ra0fHUBAXf986ss5zrmJd4CZQI__usnW-DMG2HCekOnysPJStkfpVgEVzHs065JSbfetDaeDTyYh9jP3YR3BsQ&amp;recommendedFlavor=JOB_SEEKER_QUALIFIED&amp;refId=15b1cd06-6373-48b2-a35c-30d598eb528e&amp;trk=d_flagship3_search_srp_jobs</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/jobs/view/1783547525/?eBP=NotAvailableFromVoyagerAPI&amp;recommendedFlavor=SCHOOL_RECRUIT&amp;refId=15b1cd06-6373-48b2-a35c-30d598eb528e&amp;trk=d_flagship3_search_srp_jobs</t>
-  </si>
-  <si>
-    <t>https://www.workopolis.com/jobsearch/viewjob/xH0kANch7dKy94S4YMzFBDc219WPcDIp9hLIYULjtZc--iZRhTSVPQ?ak=software+developer&amp;l=Toronto%2C+ON&amp;isp=1</t>
   </si>
   <si>
     <t>Date</t>
@@ -122,6 +65,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -191,12 +137,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -501,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -514,164 +461,1061 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
+      <c r="B2" s="3">
+        <v>43987</v>
       </c>
       <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>0</v>
+      <c r="B3" s="3">
+        <v>43989</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
+      <c r="B4" s="3">
+        <v>43989</v>
       </c>
       <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>0</v>
+      <c r="B5" s="3">
+        <v>43990</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>0</v>
+      <c r="B6" s="3">
+        <v>43990</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>0</v>
+      <c r="B7" s="3">
+        <v>43990</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="B13" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="B15" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="B22" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
+      <c r="B28" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C44" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:F7">
+  <conditionalFormatting sqref="C1:F46">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Not found">
       <formula>NOT(ISERROR(SEARCH("Not found",C1)))</formula>
     </cfRule>
@@ -683,6 +1527,45 @@
     <hyperlink ref="G5" r:id="rId4"/>
     <hyperlink ref="G6" r:id="rId5"/>
     <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G8" r:id="rId7"/>
+    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G10" r:id="rId9"/>
+    <hyperlink ref="G11" r:id="rId10"/>
+    <hyperlink ref="G12" r:id="rId11"/>
+    <hyperlink ref="G13" r:id="rId12"/>
+    <hyperlink ref="G14" r:id="rId13"/>
+    <hyperlink ref="G15" r:id="rId14"/>
+    <hyperlink ref="G16" r:id="rId15"/>
+    <hyperlink ref="G17" r:id="rId16"/>
+    <hyperlink ref="G18" r:id="rId17"/>
+    <hyperlink ref="G19" r:id="rId18"/>
+    <hyperlink ref="G20" r:id="rId19"/>
+    <hyperlink ref="G21" r:id="rId20"/>
+    <hyperlink ref="G22" r:id="rId21"/>
+    <hyperlink ref="G23" r:id="rId22"/>
+    <hyperlink ref="G24" r:id="rId23"/>
+    <hyperlink ref="G25" r:id="rId24"/>
+    <hyperlink ref="G26" r:id="rId25"/>
+    <hyperlink ref="G27" r:id="rId26"/>
+    <hyperlink ref="G28" r:id="rId27"/>
+    <hyperlink ref="G29" r:id="rId28"/>
+    <hyperlink ref="G30" r:id="rId29"/>
+    <hyperlink ref="G31" r:id="rId30"/>
+    <hyperlink ref="G32" r:id="rId31"/>
+    <hyperlink ref="G33" r:id="rId32"/>
+    <hyperlink ref="G34" r:id="rId33"/>
+    <hyperlink ref="G35" r:id="rId34"/>
+    <hyperlink ref="G36" r:id="rId35"/>
+    <hyperlink ref="G37" r:id="rId36"/>
+    <hyperlink ref="G38" r:id="rId37"/>
+    <hyperlink ref="G39" r:id="rId38"/>
+    <hyperlink ref="G40" r:id="rId39"/>
+    <hyperlink ref="G41" r:id="rId40"/>
+    <hyperlink ref="G42" r:id="rId41"/>
+    <hyperlink ref="G43" r:id="rId42"/>
+    <hyperlink ref="G44" r:id="rId43"/>
+    <hyperlink ref="G45" r:id="rId44"/>
+    <hyperlink ref="G46" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented skills distribution analysis
</commit_message>
<xml_diff>
--- a/Applications.xlsx
+++ b/Applications.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="15">
   <si>
     <t>Web Developer Intern</t>
   </si>
@@ -448,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1514,8 +1514,192 @@
         <v>8</v>
       </c>
     </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C48" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3">
+        <v>43990</v>
+      </c>
+      <c r="C50" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3">
+        <v>43991</v>
+      </c>
+      <c r="C51" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3">
+        <v>43991</v>
+      </c>
+      <c r="C52" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="3">
+        <v>43991</v>
+      </c>
+      <c r="C53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" s="3">
+        <v>43991</v>
+      </c>
+      <c r="C54" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:F46">
+  <conditionalFormatting sqref="C1:F54">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Not found">
       <formula>NOT(ISERROR(SEARCH("Not found",C1)))</formula>
     </cfRule>
@@ -1566,6 +1750,14 @@
     <hyperlink ref="G44" r:id="rId43"/>
     <hyperlink ref="G45" r:id="rId44"/>
     <hyperlink ref="G46" r:id="rId45"/>
+    <hyperlink ref="G47" r:id="rId46"/>
+    <hyperlink ref="G48" r:id="rId47"/>
+    <hyperlink ref="G49" r:id="rId48"/>
+    <hyperlink ref="G50" r:id="rId49"/>
+    <hyperlink ref="G51" r:id="rId50"/>
+    <hyperlink ref="G52" r:id="rId51"/>
+    <hyperlink ref="G53" r:id="rId52"/>
+    <hyperlink ref="G54" r:id="rId53"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>